<commit_message>
Flex Sensor and Stepper Motor Kit
</commit_message>
<xml_diff>
--- a/ISTEM2023/PartsList.xlsx
+++ b/ISTEM2023/PartsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leistimo\Documents\GitHub\Breadboard-Powersupply Book\ISTEM2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78807DFF-0AD9-4BD5-BE70-06E3D4BDF747}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A7E575-0151-4C30-87F3-1F17D00CCA39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{BFFB1414-B767-401C-B7C3-C25E65320134}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Bread Board Power Supply Kit</t>
   </si>
@@ -60,18 +60,9 @@
     <t>One Each</t>
   </si>
   <si>
-    <t>Resistor Kit</t>
-  </si>
-  <si>
-    <t>LED Kit</t>
-  </si>
-  <si>
     <t>Piezo Buzzer Set</t>
   </si>
   <si>
-    <t xml:space="preserve">Momentary Switch </t>
-  </si>
-  <si>
     <t>Potentiometer Set</t>
   </si>
   <si>
@@ -82,6 +73,18 @@
   </si>
   <si>
     <t>Blue Tooth modules</t>
+  </si>
+  <si>
+    <t>Electronics Components Kit</t>
+  </si>
+  <si>
+    <t>Momentary Switch Set</t>
+  </si>
+  <si>
+    <t>Flex Sensor</t>
+  </si>
+  <si>
+    <t>Stepper Motor kit</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +504,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -567,77 +570,88 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="1">
-        <v>8.99</v>
+        <v>36.99</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1">
-        <v>9.99</v>
+        <v>5.49</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="1">
-        <v>5.49</v>
+        <v>8.99</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="1">
-        <v>8.99</v>
+        <v>12.99</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="1">
-        <v>12.99</v>
+        <v>7.99</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="1">
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+        <v>7.97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>14.59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1">
-        <f>SUM(C2:C16)</f>
-        <v>196.86000000000004</v>
+        <f>SUM(C2:C17)</f>
+        <v>237.43000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -649,15 +663,16 @@
     <hyperlink ref="B9" r:id="rId5" xr:uid="{F616D960-AAF7-4E45-9FD6-AB6FECF67177}"/>
     <hyperlink ref="B10" r:id="rId6" xr:uid="{B1985C6A-5246-4C10-8ED4-5C0F4BF05D01}"/>
     <hyperlink ref="B6" r:id="rId7" xr:uid="{65B0DBF4-94C7-4FEC-81CC-EBA0DDC4360C}"/>
-    <hyperlink ref="B11" r:id="rId8" xr:uid="{7D7CE644-44D5-453F-ABEE-CF7C8E3DC469}"/>
-    <hyperlink ref="B12" r:id="rId9" xr:uid="{5815C1B4-51A5-48A1-9C1A-2989AAE90A84}"/>
-    <hyperlink ref="B13" r:id="rId10" xr:uid="{AA76B15C-62DC-4D18-B265-D3DE5FA46C35}"/>
-    <hyperlink ref="B14" r:id="rId11" xr:uid="{4AECC9BE-CDFC-4C58-985E-5D00D914F124}"/>
-    <hyperlink ref="B15" r:id="rId12" xr:uid="{891FE454-9879-49E9-9C30-A0BD8222664C}"/>
-    <hyperlink ref="B16" r:id="rId13" xr:uid="{52484A7B-35DB-4C1F-AFB6-0A9B0B463EC0}"/>
-    <hyperlink ref="B5" r:id="rId14" xr:uid="{E87BA6E7-4674-4C10-811A-DA1313E18548}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{AA76B15C-62DC-4D18-B265-D3DE5FA46C35}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{4AECC9BE-CDFC-4C58-985E-5D00D914F124}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{891FE454-9879-49E9-9C30-A0BD8222664C}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{52484A7B-35DB-4C1F-AFB6-0A9B0B463EC0}"/>
+    <hyperlink ref="B5" r:id="rId12" xr:uid="{E87BA6E7-4674-4C10-811A-DA1313E18548}"/>
+    <hyperlink ref="B11" r:id="rId13" xr:uid="{28E92D61-7E56-4255-AA32-1D6AB7391B9C}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{BB81A642-1D68-4FD9-99BE-4A395DB0F54F}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{3346062F-560A-499D-B835-6E518E07D7E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated Excel for ISTEM
</commit_message>
<xml_diff>
--- a/ISTEM2023/PartsList.xlsx
+++ b/ISTEM2023/PartsList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leistimo\Documents\GitHub\Breadboard-Powersupply Book\ISTEM2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A7E575-0151-4C30-87F3-1F17D00CCA39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D07F0B1-C5C2-4DA0-8253-54F41DA46F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{BFFB1414-B767-401C-B7C3-C25E65320134}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BFFB1414-B767-401C-B7C3-C25E65320134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>Bread Board Power Supply Kit</t>
   </si>
@@ -45,9 +54,6 @@
     <t>Digital Multimeter plus accessory kit</t>
   </si>
   <si>
-    <t>Arduino 37 in 1 Sensor Kit</t>
-  </si>
-  <si>
     <t>Breadboard Jumper wire kit</t>
   </si>
   <si>
@@ -60,9 +66,6 @@
     <t>One Each</t>
   </si>
   <si>
-    <t>Piezo Buzzer Set</t>
-  </si>
-  <si>
     <t>Potentiometer Set</t>
   </si>
   <si>
@@ -85,6 +88,21 @@
   </si>
   <si>
     <t>Stepper Motor kit</t>
+  </si>
+  <si>
+    <t>Received For Content Development</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Arduino 37 in 1 Sensor Kit (not available)</t>
+  </si>
+  <si>
+    <t>Arduino Sensor Kit 48 Sensor</t>
+  </si>
+  <si>
+    <t>Piezo Buzzer Set (unavailable)</t>
   </si>
 </sst>
 </file>
@@ -451,25 +469,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA27EC04-3514-4854-8B92-29ACDBB45E3E}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="30.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -480,7 +502,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -490,189 +512,240 @@
       <c r="C3" s="1">
         <v>7.99</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>23.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>54.98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>15.49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>24.99</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>11.99</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>23.99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6.98</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9.99</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>36.99</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>15.49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>24.99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>11.99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>6.98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1">
-        <v>9.99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5.49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>12.99</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>7.99</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1">
-        <v>36.99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>7.97</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1">
-        <v>5.49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1">
-        <v>8.99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>14.59</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="1">
-        <v>12.99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="1">
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1">
-        <v>7.97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1">
-        <v>14.59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="1">
-        <f>SUM(C2:C17)</f>
-        <v>237.43000000000004</v>
+      <c r="C19" s="1">
+        <f>SUM(C2:C18)</f>
+        <v>259.43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{D8FEF306-B2E5-4085-9F12-140F2A19F888}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{6C21AAC8-DFB8-477D-B5B7-DB8847EBFFB6}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{EB249100-1776-4B4F-8AF5-FDD4030BC228}"/>
-    <hyperlink ref="B8" r:id="rId4" xr:uid="{B9F70AFB-6032-4664-A1B6-27FC6826580D}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{F616D960-AAF7-4E45-9FD6-AB6FECF67177}"/>
-    <hyperlink ref="B10" r:id="rId6" xr:uid="{B1985C6A-5246-4C10-8ED4-5C0F4BF05D01}"/>
-    <hyperlink ref="B6" r:id="rId7" xr:uid="{65B0DBF4-94C7-4FEC-81CC-EBA0DDC4360C}"/>
-    <hyperlink ref="B12" r:id="rId8" xr:uid="{AA76B15C-62DC-4D18-B265-D3DE5FA46C35}"/>
-    <hyperlink ref="B13" r:id="rId9" xr:uid="{4AECC9BE-CDFC-4C58-985E-5D00D914F124}"/>
-    <hyperlink ref="B14" r:id="rId10" xr:uid="{891FE454-9879-49E9-9C30-A0BD8222664C}"/>
-    <hyperlink ref="B15" r:id="rId11" xr:uid="{52484A7B-35DB-4C1F-AFB6-0A9B0B463EC0}"/>
-    <hyperlink ref="B5" r:id="rId12" xr:uid="{E87BA6E7-4674-4C10-811A-DA1313E18548}"/>
-    <hyperlink ref="B11" r:id="rId13" xr:uid="{28E92D61-7E56-4255-AA32-1D6AB7391B9C}"/>
-    <hyperlink ref="B16" r:id="rId14" xr:uid="{BB81A642-1D68-4FD9-99BE-4A395DB0F54F}"/>
-    <hyperlink ref="B17" r:id="rId15" xr:uid="{3346062F-560A-499D-B835-6E518E07D7E0}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{EB249100-1776-4B4F-8AF5-FDD4030BC228}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{B9F70AFB-6032-4664-A1B6-27FC6826580D}"/>
+    <hyperlink ref="B10" r:id="rId5" xr:uid="{F616D960-AAF7-4E45-9FD6-AB6FECF67177}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{B1985C6A-5246-4C10-8ED4-5C0F4BF05D01}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{65B0DBF4-94C7-4FEC-81CC-EBA0DDC4360C}"/>
+    <hyperlink ref="B13" r:id="rId8" xr:uid="{AA76B15C-62DC-4D18-B265-D3DE5FA46C35}"/>
+    <hyperlink ref="B14" r:id="rId9" xr:uid="{4AECC9BE-CDFC-4C58-985E-5D00D914F124}"/>
+    <hyperlink ref="B15" r:id="rId10" xr:uid="{891FE454-9879-49E9-9C30-A0BD8222664C}"/>
+    <hyperlink ref="B16" r:id="rId11" xr:uid="{52484A7B-35DB-4C1F-AFB6-0A9B0B463EC0}"/>
+    <hyperlink ref="B6" r:id="rId12" xr:uid="{E87BA6E7-4674-4C10-811A-DA1313E18548}"/>
+    <hyperlink ref="B12" r:id="rId13" xr:uid="{28E92D61-7E56-4255-AA32-1D6AB7391B9C}"/>
+    <hyperlink ref="B17" r:id="rId14" xr:uid="{BB81A642-1D68-4FD9-99BE-4A395DB0F54F}"/>
+    <hyperlink ref="B18" r:id="rId15" xr:uid="{3346062F-560A-499D-B835-6E518E07D7E0}"/>
+    <hyperlink ref="B5" r:id="rId16" xr:uid="{5C31F98E-BDAA-42AA-B61F-4919635BE025}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>